<commit_message>
toevoegingen PROG-III en PROG-IV
</commit_message>
<xml_diff>
--- a/document/Portfoliomatrix_v100.xlsx
+++ b/document/Portfoliomatrix_v100.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\hu-repos\AI-S2_student\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D24B6E6-0903-4AE2-974A-1C4B7A17DB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4959FCCE-1F51-48FC-966C-1D2C6153F5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="2640" windowWidth="28740" windowHeight="15350" xr2:uid="{9145D055-8147-4D48-BED2-085A2CF38ACC}"/>
+    <workbookView xWindow="4460" yWindow="2910" windowWidth="28740" windowHeight="15350" xr2:uid="{9145D055-8147-4D48-BED2-085A2CF38ACC}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio-Matrix .. Semester .." sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
   <si>
     <t>Portfoliomatrix - Artificial Intelligence - Semester 2</t>
   </si>
@@ -400,6 +400,9 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>18/03/2025</t>
+  </si>
 </sst>
 </file>
 
@@ -1421,6 +1424,117 @@
     <xf numFmtId="0" fontId="6" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1442,12 +1556,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1493,110 +1601,17 @@
     <xf numFmtId="0" fontId="5" fillId="19" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1621,18 +1636,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4652,9 +4655,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4692,7 +4695,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4798,7 +4801,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4940,7 +4943,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4953,8 +4956,8 @@
   </sheetPr>
   <dimension ref="A1:AT36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5113,64 +5116,64 @@
         <v>2</v>
       </c>
       <c r="D4" s="80"/>
-      <c r="E4" s="121" t="s">
+      <c r="E4" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="G4" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="118" t="s">
+      <c r="H4" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="118" t="s">
+      <c r="I4" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="118" t="s">
+      <c r="J4" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="118" t="s">
+      <c r="K4" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="118" t="s">
+      <c r="L4" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="115" t="s">
+      <c r="M4" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="115" t="s">
+      <c r="N4" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="115" t="s">
+      <c r="O4" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="115" t="s">
+      <c r="P4" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="115" t="s">
+      <c r="Q4" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="115" t="s">
+      <c r="R4" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="115" t="s">
+      <c r="S4" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="106" t="s">
+      <c r="T4" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="106" t="s">
+      <c r="U4" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="106" t="s">
+      <c r="V4" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="W4" s="109" t="s">
+      <c r="W4" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="X4" s="112" t="s">
+      <c r="X4" s="147" t="s">
         <v>22</v>
       </c>
       <c r="Y4" s="65"/>
@@ -5180,22 +5183,22 @@
       <c r="AC4" s="66"/>
       <c r="AD4" s="66"/>
       <c r="AE4" s="67"/>
-      <c r="AF4" s="100" t="s">
+      <c r="AF4" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="AG4" s="103" t="s">
+      <c r="AG4" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="AH4" s="103" t="s">
+      <c r="AH4" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="AI4" s="103" t="s">
+      <c r="AI4" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="AJ4" s="103" t="s">
+      <c r="AJ4" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="AK4" s="91" t="s">
+      <c r="AK4" s="128" t="s">
         <v>28</v>
       </c>
       <c r="AL4" s="81"/>
@@ -5205,28 +5208,30 @@
       <c r="B5" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="60" t="s">
+        <v>54</v>
+      </c>
       <c r="D5" s="89"/>
-      <c r="E5" s="122"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="113"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="126"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="126"/>
+      <c r="Q5" s="126"/>
+      <c r="R5" s="126"/>
+      <c r="S5" s="126"/>
+      <c r="T5" s="142"/>
+      <c r="U5" s="142"/>
+      <c r="V5" s="142"/>
+      <c r="W5" s="145"/>
+      <c r="X5" s="148"/>
       <c r="Y5" s="68"/>
       <c r="Z5" s="69"/>
       <c r="AA5" s="69"/>
@@ -5234,12 +5239,12 @@
       <c r="AC5" s="69"/>
       <c r="AD5" s="69"/>
       <c r="AE5" s="70"/>
-      <c r="AF5" s="101"/>
-      <c r="AG5" s="104"/>
-      <c r="AH5" s="104"/>
-      <c r="AI5" s="104"/>
-      <c r="AJ5" s="104"/>
-      <c r="AK5" s="92"/>
+      <c r="AF5" s="136"/>
+      <c r="AG5" s="139"/>
+      <c r="AH5" s="139"/>
+      <c r="AI5" s="139"/>
+      <c r="AJ5" s="139"/>
+      <c r="AK5" s="129"/>
       <c r="AL5" s="81"/>
     </row>
     <row r="6" spans="1:46" s="38" customFormat="1" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5247,26 +5252,26 @@
       <c r="B6" s="85"/>
       <c r="C6" s="87"/>
       <c r="D6" s="88"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="108"/>
-      <c r="U6" s="108"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="111"/>
-      <c r="X6" s="114"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="127"/>
+      <c r="Q6" s="127"/>
+      <c r="R6" s="127"/>
+      <c r="S6" s="127"/>
+      <c r="T6" s="143"/>
+      <c r="U6" s="143"/>
+      <c r="V6" s="143"/>
+      <c r="W6" s="146"/>
+      <c r="X6" s="149"/>
       <c r="Y6" s="72" t="s">
         <v>30</v>
       </c>
@@ -5288,23 +5293,23 @@
       <c r="AE6" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="AF6" s="102"/>
-      <c r="AG6" s="105"/>
-      <c r="AH6" s="105"/>
-      <c r="AI6" s="105"/>
-      <c r="AJ6" s="105"/>
-      <c r="AK6" s="93"/>
+      <c r="AF6" s="137"/>
+      <c r="AG6" s="140"/>
+      <c r="AH6" s="140"/>
+      <c r="AI6" s="140"/>
+      <c r="AJ6" s="140"/>
+      <c r="AK6" s="130"/>
       <c r="AL6" s="85"/>
     </row>
     <row r="7" spans="1:46" ht="36" x14ac:dyDescent="0.35">
       <c r="A7" s="78"/>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="95"/>
+      <c r="D7" s="132"/>
       <c r="E7" s="40"/>
       <c r="F7" s="35"/>
       <c r="G7" s="90" t="s">
@@ -5312,7 +5317,9 @@
       </c>
       <c r="H7" s="35"/>
       <c r="I7" s="12"/>
-      <c r="J7" s="35"/>
+      <c r="J7" s="90" t="s">
+        <v>41</v>
+      </c>
       <c r="K7" s="12"/>
       <c r="L7" s="35"/>
       <c r="M7" s="12"/>
@@ -5350,18 +5357,22 @@
     </row>
     <row r="8" spans="1:46" ht="36" x14ac:dyDescent="0.35">
       <c r="A8" s="78"/>
-      <c r="B8" s="138"/>
-      <c r="C8" s="96" t="s">
+      <c r="B8" s="95"/>
+      <c r="C8" s="133" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="97"/>
+      <c r="D8" s="134"/>
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="32"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
+      <c r="J8" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="90" t="s">
+        <v>41</v>
+      </c>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="17"/>
@@ -5398,11 +5409,11 @@
     </row>
     <row r="9" spans="1:46" ht="36" x14ac:dyDescent="0.35">
       <c r="A9" s="78"/>
-      <c r="B9" s="138"/>
-      <c r="C9" s="98" t="s">
+      <c r="B9" s="95"/>
+      <c r="C9" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="99"/>
+      <c r="D9" s="98"/>
       <c r="E9" s="90" t="s">
         <v>41</v>
       </c>
@@ -5448,11 +5459,11 @@
     </row>
     <row r="10" spans="1:46" ht="36" x14ac:dyDescent="0.35">
       <c r="A10" s="78"/>
-      <c r="B10" s="138"/>
-      <c r="C10" s="98" t="s">
+      <c r="B10" s="95"/>
+      <c r="C10" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="99"/>
+      <c r="D10" s="98"/>
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -5498,11 +5509,11 @@
     </row>
     <row r="11" spans="1:46" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="78"/>
-      <c r="B11" s="138"/>
-      <c r="C11" s="98" t="s">
+      <c r="B11" s="95"/>
+      <c r="C11" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="99"/>
+      <c r="D11" s="98"/>
       <c r="E11" s="15"/>
       <c r="F11" s="44"/>
       <c r="G11" s="14"/>
@@ -5546,11 +5557,11 @@
     </row>
     <row r="12" spans="1:46" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="78"/>
-      <c r="B12" s="139"/>
-      <c r="C12" s="140" t="s">
+      <c r="B12" s="96"/>
+      <c r="C12" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="141"/>
+      <c r="D12" s="100"/>
       <c r="E12" s="46"/>
       <c r="F12" s="47"/>
       <c r="G12" s="47"/>
@@ -5594,13 +5605,13 @@
     </row>
     <row r="13" spans="1:46" ht="36" x14ac:dyDescent="0.8">
       <c r="A13" s="78"/>
-      <c r="B13" s="134" t="s">
+      <c r="B13" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="142" t="s">
+      <c r="C13" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="143"/>
+      <c r="D13" s="102"/>
       <c r="E13" s="62"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
@@ -5644,11 +5655,11 @@
     </row>
     <row r="14" spans="1:46" ht="36" x14ac:dyDescent="0.8">
       <c r="A14" s="78"/>
-      <c r="B14" s="135"/>
-      <c r="C14" s="144" t="s">
+      <c r="B14" s="92"/>
+      <c r="C14" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="145"/>
+      <c r="D14" s="104"/>
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
@@ -5692,11 +5703,11 @@
     </row>
     <row r="15" spans="1:46" ht="36" x14ac:dyDescent="0.8">
       <c r="A15" s="78"/>
-      <c r="B15" s="135"/>
-      <c r="C15" s="146" t="s">
+      <c r="B15" s="92"/>
+      <c r="C15" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="147"/>
+      <c r="D15" s="106"/>
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
@@ -5740,11 +5751,11 @@
     </row>
     <row r="16" spans="1:46" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="A16" s="78"/>
-      <c r="B16" s="136"/>
-      <c r="C16" s="148" t="s">
+      <c r="B16" s="93"/>
+      <c r="C16" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="149"/>
+      <c r="D16" s="108"/>
       <c r="E16" s="29"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
@@ -5867,83 +5878,83 @@
       <c r="AL18" s="81"/>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="G21" s="130"/>
-      <c r="H21" s="126" t="s">
+      <c r="G21" s="115"/>
+      <c r="H21" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="127"/>
-      <c r="J21" s="127"/>
-      <c r="K21" s="127"/>
-      <c r="L21" s="127"/>
-      <c r="M21" s="127"/>
-      <c r="N21" s="127"/>
-      <c r="O21" s="127"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="112"/>
+      <c r="M21" s="112"/>
+      <c r="N21" s="112"/>
+      <c r="O21" s="112"/>
       <c r="P21" s="76"/>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="G22" s="131"/>
-      <c r="H22" s="126"/>
-      <c r="I22" s="127"/>
-      <c r="J22" s="127"/>
-      <c r="K22" s="127"/>
-      <c r="L22" s="127"/>
-      <c r="M22" s="127"/>
-      <c r="N22" s="127"/>
-      <c r="O22" s="127"/>
+      <c r="G22" s="116"/>
+      <c r="H22" s="111"/>
+      <c r="I22" s="112"/>
+      <c r="J22" s="112"/>
+      <c r="K22" s="112"/>
+      <c r="L22" s="112"/>
+      <c r="M22" s="112"/>
+      <c r="N22" s="112"/>
+      <c r="O22" s="112"/>
       <c r="P22" s="76"/>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="G24" s="124"/>
-      <c r="H24" s="126" t="s">
+      <c r="G24" s="109"/>
+      <c r="H24" s="111" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="127"/>
-      <c r="J24" s="127"/>
-      <c r="K24" s="127"/>
-      <c r="L24" s="127"/>
-      <c r="M24" s="127"/>
-      <c r="N24" s="127"/>
-      <c r="O24" s="127"/>
+      <c r="I24" s="112"/>
+      <c r="J24" s="112"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="112"/>
+      <c r="M24" s="112"/>
+      <c r="N24" s="112"/>
+      <c r="O24" s="112"/>
       <c r="P24" s="76"/>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="G25" s="125"/>
-      <c r="H25" s="126"/>
-      <c r="I25" s="127"/>
-      <c r="J25" s="127"/>
-      <c r="K25" s="127"/>
-      <c r="L25" s="127"/>
-      <c r="M25" s="127"/>
-      <c r="N25" s="127"/>
-      <c r="O25" s="127"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="111"/>
+      <c r="I25" s="112"/>
+      <c r="J25" s="112"/>
+      <c r="K25" s="112"/>
+      <c r="L25" s="112"/>
+      <c r="M25" s="112"/>
+      <c r="N25" s="112"/>
+      <c r="O25" s="112"/>
       <c r="P25" s="76"/>
     </row>
     <row r="27" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G27" s="132" t="s">
+      <c r="G27" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="128" t="s">
+      <c r="H27" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="I27" s="129"/>
-      <c r="J27" s="129"/>
-      <c r="K27" s="129"/>
-      <c r="L27" s="129"/>
-      <c r="M27" s="129"/>
-      <c r="N27" s="129"/>
-      <c r="O27" s="129"/>
+      <c r="I27" s="114"/>
+      <c r="J27" s="114"/>
+      <c r="K27" s="114"/>
+      <c r="L27" s="114"/>
+      <c r="M27" s="114"/>
+      <c r="N27" s="114"/>
+      <c r="O27" s="114"/>
       <c r="P27" s="77"/>
     </row>
     <row r="28" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G28" s="133"/>
-      <c r="H28" s="128"/>
-      <c r="I28" s="129"/>
-      <c r="J28" s="129"/>
-      <c r="K28" s="129"/>
-      <c r="L28" s="129"/>
-      <c r="M28" s="129"/>
-      <c r="N28" s="129"/>
-      <c r="O28" s="129"/>
+      <c r="G28" s="118"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="114"/>
+      <c r="J28" s="114"/>
+      <c r="K28" s="114"/>
+      <c r="L28" s="114"/>
+      <c r="M28" s="114"/>
+      <c r="N28" s="114"/>
+      <c r="O28" s="114"/>
       <c r="P28" s="77"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.35">
@@ -5978,34 +5989,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:O25"/>
-    <mergeCell ref="H27:O28"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:O22"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="S4:S6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="N4:N6"/>
     <mergeCell ref="AK4:AK6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
@@ -6022,6 +6005,34 @@
     <mergeCell ref="W4:W6"/>
     <mergeCell ref="X4:X6"/>
     <mergeCell ref="O4:O6"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="Q4:Q6"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:O25"/>
+    <mergeCell ref="H27:O28"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:O22"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" verticalDpi="1200" r:id="rId1"/>
@@ -6158,64 +6169,64 @@
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="71"/>
-      <c r="E4" s="121" t="s">
+      <c r="E4" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="G4" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="118" t="s">
+      <c r="H4" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="118" t="s">
+      <c r="I4" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="118" t="s">
+      <c r="J4" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="118" t="s">
+      <c r="K4" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="118" t="s">
+      <c r="L4" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="115" t="s">
+      <c r="M4" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="115" t="s">
+      <c r="N4" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="115" t="s">
+      <c r="O4" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="115" t="s">
+      <c r="P4" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="115" t="s">
+      <c r="Q4" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="115" t="s">
+      <c r="R4" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="115" t="s">
+      <c r="S4" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="106" t="s">
+      <c r="T4" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="106" t="s">
+      <c r="U4" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="106" t="s">
+      <c r="V4" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="W4" s="109" t="s">
+      <c r="W4" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="X4" s="112" t="s">
+      <c r="X4" s="147" t="s">
         <v>22</v>
       </c>
       <c r="Y4" s="65"/>
@@ -6225,22 +6236,22 @@
       <c r="AC4" s="66"/>
       <c r="AD4" s="66"/>
       <c r="AE4" s="67"/>
-      <c r="AF4" s="100" t="s">
+      <c r="AF4" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="AG4" s="103" t="s">
+      <c r="AG4" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="AH4" s="103" t="s">
+      <c r="AH4" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="AI4" s="103" t="s">
+      <c r="AI4" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="AJ4" s="103" t="s">
+      <c r="AJ4" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="AK4" s="91" t="s">
+      <c r="AK4" s="128" t="s">
         <v>28</v>
       </c>
     </row>
@@ -6250,26 +6261,26 @@
       </c>
       <c r="C5" s="60"/>
       <c r="D5" s="63"/>
-      <c r="E5" s="122"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="113"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="126"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="126"/>
+      <c r="Q5" s="126"/>
+      <c r="R5" s="126"/>
+      <c r="S5" s="126"/>
+      <c r="T5" s="142"/>
+      <c r="U5" s="142"/>
+      <c r="V5" s="142"/>
+      <c r="W5" s="145"/>
+      <c r="X5" s="148"/>
       <c r="Y5" s="68"/>
       <c r="Z5" s="69"/>
       <c r="AA5" s="69"/>
@@ -6277,37 +6288,37 @@
       <c r="AC5" s="69"/>
       <c r="AD5" s="69"/>
       <c r="AE5" s="70"/>
-      <c r="AF5" s="101"/>
-      <c r="AG5" s="104"/>
-      <c r="AH5" s="104"/>
-      <c r="AI5" s="104"/>
-      <c r="AJ5" s="104"/>
-      <c r="AK5" s="92"/>
+      <c r="AF5" s="136"/>
+      <c r="AG5" s="139"/>
+      <c r="AH5" s="139"/>
+      <c r="AI5" s="139"/>
+      <c r="AJ5" s="139"/>
+      <c r="AK5" s="129"/>
     </row>
     <row r="6" spans="2:37" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="38"/>
       <c r="C6" s="64"/>
       <c r="D6" s="34"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="108"/>
-      <c r="U6" s="108"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="111"/>
-      <c r="X6" s="114"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="127"/>
+      <c r="Q6" s="127"/>
+      <c r="R6" s="127"/>
+      <c r="S6" s="127"/>
+      <c r="T6" s="143"/>
+      <c r="U6" s="143"/>
+      <c r="V6" s="143"/>
+      <c r="W6" s="146"/>
+      <c r="X6" s="149"/>
       <c r="Y6" s="72" t="s">
         <v>30</v>
       </c>
@@ -6329,21 +6340,21 @@
       <c r="AE6" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="AF6" s="102"/>
-      <c r="AG6" s="105"/>
-      <c r="AH6" s="105"/>
-      <c r="AI6" s="105"/>
-      <c r="AJ6" s="105"/>
-      <c r="AK6" s="93"/>
+      <c r="AF6" s="137"/>
+      <c r="AG6" s="140"/>
+      <c r="AH6" s="140"/>
+      <c r="AI6" s="140"/>
+      <c r="AJ6" s="140"/>
+      <c r="AK6" s="130"/>
     </row>
     <row r="7" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="150" t="s">
+      <c r="C7" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="151"/>
+      <c r="D7" s="155"/>
       <c r="E7" s="40"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
@@ -6379,11 +6390,11 @@
       <c r="AK7" s="7"/>
     </row>
     <row r="8" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="138"/>
-      <c r="C8" s="152" t="s">
+      <c r="B8" s="95"/>
+      <c r="C8" s="156" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="153"/>
+      <c r="D8" s="157"/>
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -6419,11 +6430,11 @@
       <c r="AK8" s="9"/>
     </row>
     <row r="9" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="138"/>
-      <c r="C9" s="154" t="s">
+      <c r="B9" s="95"/>
+      <c r="C9" s="158" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="155"/>
+      <c r="D9" s="159"/>
       <c r="E9" s="45"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -6459,11 +6470,11 @@
       <c r="AK9" s="9"/>
     </row>
     <row r="10" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="138"/>
-      <c r="C10" s="154" t="s">
+      <c r="B10" s="95"/>
+      <c r="C10" s="158" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="155"/>
+      <c r="D10" s="159"/>
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -6499,11 +6510,11 @@
       <c r="AK10" s="9"/>
     </row>
     <row r="11" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="138"/>
-      <c r="C11" s="154" t="s">
+      <c r="B11" s="95"/>
+      <c r="C11" s="158" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="155"/>
+      <c r="D11" s="159"/>
       <c r="E11" s="15"/>
       <c r="F11" s="44"/>
       <c r="G11" s="14"/>
@@ -6539,11 +6550,11 @@
       <c r="AK11" s="9"/>
     </row>
     <row r="12" spans="2:37" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="139"/>
-      <c r="C12" s="156" t="s">
+      <c r="B12" s="96"/>
+      <c r="C12" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="157"/>
+      <c r="D12" s="161"/>
       <c r="E12" s="46"/>
       <c r="F12" s="47"/>
       <c r="G12" s="47"/>
@@ -6579,13 +6590,13 @@
       <c r="AK12" s="18"/>
     </row>
     <row r="13" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B13" s="134" t="s">
+      <c r="B13" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="158" t="s">
+      <c r="C13" s="150" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="159"/>
+      <c r="D13" s="151"/>
       <c r="E13" s="62"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
@@ -6621,11 +6632,11 @@
       <c r="AK13" s="27"/>
     </row>
     <row r="14" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B14" s="135"/>
-      <c r="C14" s="160" t="s">
+      <c r="B14" s="92"/>
+      <c r="C14" s="152" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="161"/>
+      <c r="D14" s="153"/>
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
@@ -6661,11 +6672,11 @@
       <c r="AK14" s="28"/>
     </row>
     <row r="15" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B15" s="135"/>
-      <c r="C15" s="146" t="s">
+      <c r="B15" s="92"/>
+      <c r="C15" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="147"/>
+      <c r="D15" s="106"/>
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
@@ -6701,11 +6712,11 @@
       <c r="AK15" s="28"/>
     </row>
     <row r="16" spans="2:37" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="B16" s="136"/>
-      <c r="C16" s="148" t="s">
+      <c r="B16" s="93"/>
+      <c r="C16" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="149"/>
+      <c r="D16" s="108"/>
       <c r="E16" s="29"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
@@ -6742,11 +6753,23 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="T4:T6"/>
+    <mergeCell ref="U4:U6"/>
+    <mergeCell ref="V4:V6"/>
     <mergeCell ref="AJ4:AJ6"/>
     <mergeCell ref="AK4:AK6"/>
     <mergeCell ref="B7:B12"/>
@@ -6763,23 +6786,11 @@
     <mergeCell ref="AH4:AH6"/>
     <mergeCell ref="AI4:AI6"/>
     <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="S4:S6"/>
-    <mergeCell ref="T4:T6"/>
-    <mergeCell ref="U4:U6"/>
-    <mergeCell ref="V4:V6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="N4:N6"/>
-    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7153,6 +7164,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="cc018f0f-33de-4c4c-920d-26dc6e1acc33" xsi:nil="true"/>
+    <test xmlns="8e39aab0-005d-45b6-a80e-05e5df2908d1" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8e39aab0-005d-45b6-a80e-05e5df2908d1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010081A80706761E274FBF7207A6EEFD509E" ma:contentTypeVersion="20" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="a00a05fe2e076f083d323378c5165ffd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8e39aab0-005d-45b6-a80e-05e5df2908d1" xmlns:ns3="cc018f0f-33de-4c4c-920d-26dc6e1acc33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64bb212a3759e4adb139958771eb6e76" ns2:_="" ns3:_="">
     <xsd:import namespace="8e39aab0-005d-45b6-a80e-05e5df2908d1"/>
@@ -7415,28 +7447,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA41F33-D73A-4946-89E5-437EF57CC713}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cc018f0f-33de-4c4c-920d-26dc6e1acc33"/>
+    <ds:schemaRef ds:uri="8e39aab0-005d-45b6-a80e-05e5df2908d1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="cc018f0f-33de-4c4c-920d-26dc6e1acc33" xsi:nil="true"/>
-    <test xmlns="8e39aab0-005d-45b6-a80e-05e5df2908d1" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8e39aab0-005d-45b6-a80e-05e5df2908d1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FEB2382-117C-4B02-B61B-7207F73C69D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0F5F45-92AD-4EE8-ADF4-74DBCD118A57}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7453,23 +7483,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FEB2382-117C-4B02-B61B-7207F73C69D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA41F33-D73A-4946-89E5-437EF57CC713}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cc018f0f-33de-4c4c-920d-26dc6e1acc33"/>
-    <ds:schemaRef ds:uri="8e39aab0-005d-45b6-a80e-05e5df2908d1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
PROG_VI toegevoed voor peilmoment 2
</commit_message>
<xml_diff>
--- a/document/Portfoliomatrix_v100.xlsx
+++ b/document/Portfoliomatrix_v100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\hu\repos\AI-S2_student\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AEDA0C-FAC9-4512-A8FB-F316D025DDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF1FCDB-BE81-4C1F-B152-5AF5764301BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="7995" windowWidth="29040" windowHeight="15720" xr2:uid="{9145D055-8147-4D48-BED2-085A2CF38ACC}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="55">
   <si>
     <t>Portfoliomatrix - Artificial Intelligence - Semester 2</t>
   </si>
@@ -1431,6 +1431,120 @@
     <xf numFmtId="0" fontId="6" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1452,12 +1566,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1503,110 +1611,17 @@
     <xf numFmtId="0" fontId="5" fillId="19" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1632,26 +1647,11 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1689,7 +1689,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>38855</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>31061</xdr:rowOff>
+      <xdr:rowOff>27886</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1752,7 +1752,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>259820</xdr:colOff>
+      <xdr:colOff>256645</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>187494</xdr:rowOff>
     </xdr:to>
@@ -4967,7 +4967,7 @@
   <dimension ref="A1:AT36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5126,64 +5126,64 @@
         <v>2</v>
       </c>
       <c r="D4" s="80"/>
-      <c r="E4" s="121" t="s">
+      <c r="E4" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="G4" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="118" t="s">
+      <c r="H4" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="118" t="s">
+      <c r="I4" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="118" t="s">
+      <c r="J4" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="118" t="s">
+      <c r="K4" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="118" t="s">
+      <c r="L4" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="115" t="s">
+      <c r="M4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="115" t="s">
+      <c r="N4" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="115" t="s">
+      <c r="O4" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="115" t="s">
+      <c r="P4" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="115" t="s">
+      <c r="Q4" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="115" t="s">
+      <c r="R4" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="115" t="s">
+      <c r="S4" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="106" t="s">
+      <c r="T4" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="106" t="s">
+      <c r="U4" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="106" t="s">
+      <c r="V4" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="W4" s="109" t="s">
+      <c r="W4" s="145" t="s">
         <v>21</v>
       </c>
-      <c r="X4" s="112" t="s">
+      <c r="X4" s="148" t="s">
         <v>22</v>
       </c>
       <c r="Y4" s="65"/>
@@ -5193,22 +5193,22 @@
       <c r="AC4" s="66"/>
       <c r="AD4" s="66"/>
       <c r="AE4" s="67"/>
-      <c r="AF4" s="100" t="s">
+      <c r="AF4" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="AG4" s="103" t="s">
+      <c r="AG4" s="139" t="s">
         <v>24</v>
       </c>
-      <c r="AH4" s="103" t="s">
+      <c r="AH4" s="139" t="s">
         <v>25</v>
       </c>
-      <c r="AI4" s="103" t="s">
+      <c r="AI4" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="AJ4" s="103" t="s">
+      <c r="AJ4" s="139" t="s">
         <v>27</v>
       </c>
-      <c r="AK4" s="91" t="s">
+      <c r="AK4" s="129" t="s">
         <v>28</v>
       </c>
       <c r="AL4" s="81"/>
@@ -5222,26 +5222,26 @@
         <v>54</v>
       </c>
       <c r="D5" s="89"/>
-      <c r="E5" s="122"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="113"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="124"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="127"/>
+      <c r="N5" s="127"/>
+      <c r="O5" s="127"/>
+      <c r="P5" s="127"/>
+      <c r="Q5" s="127"/>
+      <c r="R5" s="127"/>
+      <c r="S5" s="127"/>
+      <c r="T5" s="143"/>
+      <c r="U5" s="143"/>
+      <c r="V5" s="143"/>
+      <c r="W5" s="146"/>
+      <c r="X5" s="149"/>
       <c r="Y5" s="68"/>
       <c r="Z5" s="69"/>
       <c r="AA5" s="69"/>
@@ -5249,12 +5249,12 @@
       <c r="AC5" s="69"/>
       <c r="AD5" s="69"/>
       <c r="AE5" s="70"/>
-      <c r="AF5" s="101"/>
-      <c r="AG5" s="104"/>
-      <c r="AH5" s="104"/>
-      <c r="AI5" s="104"/>
-      <c r="AJ5" s="104"/>
-      <c r="AK5" s="92"/>
+      <c r="AF5" s="137"/>
+      <c r="AG5" s="140"/>
+      <c r="AH5" s="140"/>
+      <c r="AI5" s="140"/>
+      <c r="AJ5" s="140"/>
+      <c r="AK5" s="130"/>
       <c r="AL5" s="81"/>
     </row>
     <row r="6" spans="1:46" s="38" customFormat="1" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5262,26 +5262,26 @@
       <c r="B6" s="85"/>
       <c r="C6" s="87"/>
       <c r="D6" s="88"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="108"/>
-      <c r="U6" s="108"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="111"/>
-      <c r="X6" s="114"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="125"/>
+      <c r="M6" s="128"/>
+      <c r="N6" s="128"/>
+      <c r="O6" s="128"/>
+      <c r="P6" s="128"/>
+      <c r="Q6" s="128"/>
+      <c r="R6" s="128"/>
+      <c r="S6" s="128"/>
+      <c r="T6" s="144"/>
+      <c r="U6" s="144"/>
+      <c r="V6" s="144"/>
+      <c r="W6" s="147"/>
+      <c r="X6" s="150"/>
       <c r="Y6" s="72" t="s">
         <v>30</v>
       </c>
@@ -5303,23 +5303,23 @@
       <c r="AE6" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="AF6" s="102"/>
-      <c r="AG6" s="105"/>
-      <c r="AH6" s="105"/>
-      <c r="AI6" s="105"/>
-      <c r="AJ6" s="105"/>
-      <c r="AK6" s="93"/>
+      <c r="AF6" s="138"/>
+      <c r="AG6" s="141"/>
+      <c r="AH6" s="141"/>
+      <c r="AI6" s="141"/>
+      <c r="AJ6" s="141"/>
+      <c r="AK6" s="131"/>
       <c r="AL6" s="85"/>
     </row>
     <row r="7" spans="1:46" ht="36" x14ac:dyDescent="0.35">
       <c r="A7" s="78"/>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="95"/>
+      <c r="D7" s="133"/>
       <c r="E7" s="40"/>
       <c r="F7" s="35"/>
       <c r="G7" s="90" t="s">
@@ -5331,7 +5331,7 @@
         <v>41</v>
       </c>
       <c r="K7" s="12"/>
-      <c r="L7" s="164" t="s">
+      <c r="L7" s="91" t="s">
         <v>41</v>
       </c>
       <c r="M7" s="12"/>
@@ -5369,11 +5369,11 @@
     </row>
     <row r="8" spans="1:46" ht="36" x14ac:dyDescent="0.35">
       <c r="A8" s="78"/>
-      <c r="B8" s="138"/>
-      <c r="C8" s="96" t="s">
+      <c r="B8" s="96"/>
+      <c r="C8" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="97"/>
+      <c r="D8" s="135"/>
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -5387,10 +5387,12 @@
       </c>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
-      <c r="N8" s="164" t="s">
+      <c r="N8" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="17"/>
+      <c r="O8" s="91" t="s">
+        <v>41</v>
+      </c>
       <c r="P8" s="17"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="3"/>
@@ -5423,7 +5425,7 @@
     </row>
     <row r="9" spans="1:46" ht="36" x14ac:dyDescent="0.35">
       <c r="A9" s="78"/>
-      <c r="B9" s="138"/>
+      <c r="B9" s="96"/>
       <c r="C9" s="98" t="s">
         <v>40</v>
       </c>
@@ -5437,12 +5439,14 @@
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="164" t="s">
+      <c r="L9" s="91" t="s">
         <v>41</v>
       </c>
       <c r="M9" s="21"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="21"/>
+      <c r="O9" s="91" t="s">
+        <v>41</v>
+      </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
@@ -5475,7 +5479,7 @@
     </row>
     <row r="10" spans="1:46" ht="36" x14ac:dyDescent="0.35">
       <c r="A10" s="78"/>
-      <c r="B10" s="138"/>
+      <c r="B10" s="96"/>
       <c r="C10" s="98" t="s">
         <v>42</v>
       </c>
@@ -5491,10 +5495,12 @@
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
-      <c r="N10" s="164" t="s">
+      <c r="N10" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="O10" s="21"/>
+      <c r="O10" s="91" t="s">
+        <v>41</v>
+      </c>
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
       <c r="R10" s="17"/>
@@ -5527,7 +5533,7 @@
     </row>
     <row r="11" spans="1:46" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="78"/>
-      <c r="B11" s="138"/>
+      <c r="B11" s="96"/>
       <c r="C11" s="98" t="s">
         <v>43</v>
       </c>
@@ -5542,7 +5548,9 @@
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
-      <c r="O11" s="17"/>
+      <c r="O11" s="91" t="s">
+        <v>41</v>
+      </c>
       <c r="P11" s="17"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
@@ -5575,11 +5583,11 @@
     </row>
     <row r="12" spans="1:46" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="78"/>
-      <c r="B12" s="139"/>
-      <c r="C12" s="140" t="s">
+      <c r="B12" s="97"/>
+      <c r="C12" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="141"/>
+      <c r="D12" s="101"/>
       <c r="E12" s="46"/>
       <c r="F12" s="47"/>
       <c r="G12" s="47"/>
@@ -5623,13 +5631,13 @@
     </row>
     <row r="13" spans="1:46" ht="36" x14ac:dyDescent="0.8">
       <c r="A13" s="78"/>
-      <c r="B13" s="134" t="s">
+      <c r="B13" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="142" t="s">
+      <c r="C13" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="143"/>
+      <c r="D13" s="103"/>
       <c r="E13" s="62"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
@@ -5673,11 +5681,11 @@
     </row>
     <row r="14" spans="1:46" ht="36" x14ac:dyDescent="0.8">
       <c r="A14" s="78"/>
-      <c r="B14" s="135"/>
-      <c r="C14" s="144" t="s">
+      <c r="B14" s="93"/>
+      <c r="C14" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="145"/>
+      <c r="D14" s="105"/>
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
@@ -5721,11 +5729,11 @@
     </row>
     <row r="15" spans="1:46" ht="36" x14ac:dyDescent="0.8">
       <c r="A15" s="78"/>
-      <c r="B15" s="135"/>
-      <c r="C15" s="146" t="s">
+      <c r="B15" s="93"/>
+      <c r="C15" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="147"/>
+      <c r="D15" s="107"/>
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
@@ -5769,11 +5777,11 @@
     </row>
     <row r="16" spans="1:46" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="A16" s="78"/>
-      <c r="B16" s="136"/>
-      <c r="C16" s="148" t="s">
+      <c r="B16" s="94"/>
+      <c r="C16" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="149"/>
+      <c r="D16" s="109"/>
       <c r="E16" s="29"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
@@ -5896,83 +5904,83 @@
       <c r="AL18" s="81"/>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="G21" s="130"/>
-      <c r="H21" s="126" t="s">
+      <c r="G21" s="116"/>
+      <c r="H21" s="112" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="127"/>
-      <c r="J21" s="127"/>
-      <c r="K21" s="127"/>
-      <c r="L21" s="127"/>
-      <c r="M21" s="127"/>
-      <c r="N21" s="127"/>
-      <c r="O21" s="127"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="113"/>
+      <c r="L21" s="113"/>
+      <c r="M21" s="113"/>
+      <c r="N21" s="113"/>
+      <c r="O21" s="113"/>
       <c r="P21" s="76"/>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="G22" s="131"/>
-      <c r="H22" s="126"/>
-      <c r="I22" s="127"/>
-      <c r="J22" s="127"/>
-      <c r="K22" s="127"/>
-      <c r="L22" s="127"/>
-      <c r="M22" s="127"/>
-      <c r="N22" s="127"/>
-      <c r="O22" s="127"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="112"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="113"/>
+      <c r="K22" s="113"/>
+      <c r="L22" s="113"/>
+      <c r="M22" s="113"/>
+      <c r="N22" s="113"/>
+      <c r="O22" s="113"/>
       <c r="P22" s="76"/>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="G24" s="124"/>
-      <c r="H24" s="126" t="s">
+      <c r="G24" s="110"/>
+      <c r="H24" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="127"/>
-      <c r="J24" s="127"/>
-      <c r="K24" s="127"/>
-      <c r="L24" s="127"/>
-      <c r="M24" s="127"/>
-      <c r="N24" s="127"/>
-      <c r="O24" s="127"/>
+      <c r="I24" s="113"/>
+      <c r="J24" s="113"/>
+      <c r="K24" s="113"/>
+      <c r="L24" s="113"/>
+      <c r="M24" s="113"/>
+      <c r="N24" s="113"/>
+      <c r="O24" s="113"/>
       <c r="P24" s="76"/>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="G25" s="125"/>
-      <c r="H25" s="126"/>
-      <c r="I25" s="127"/>
-      <c r="J25" s="127"/>
-      <c r="K25" s="127"/>
-      <c r="L25" s="127"/>
-      <c r="M25" s="127"/>
-      <c r="N25" s="127"/>
-      <c r="O25" s="127"/>
+      <c r="G25" s="111"/>
+      <c r="H25" s="112"/>
+      <c r="I25" s="113"/>
+      <c r="J25" s="113"/>
+      <c r="K25" s="113"/>
+      <c r="L25" s="113"/>
+      <c r="M25" s="113"/>
+      <c r="N25" s="113"/>
+      <c r="O25" s="113"/>
       <c r="P25" s="76"/>
     </row>
     <row r="27" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G27" s="132" t="s">
+      <c r="G27" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="128" t="s">
+      <c r="H27" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="I27" s="129"/>
-      <c r="J27" s="129"/>
-      <c r="K27" s="129"/>
-      <c r="L27" s="129"/>
-      <c r="M27" s="129"/>
-      <c r="N27" s="129"/>
-      <c r="O27" s="129"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="115"/>
+      <c r="L27" s="115"/>
+      <c r="M27" s="115"/>
+      <c r="N27" s="115"/>
+      <c r="O27" s="115"/>
       <c r="P27" s="77"/>
     </row>
     <row r="28" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G28" s="133"/>
-      <c r="H28" s="128"/>
-      <c r="I28" s="129"/>
-      <c r="J28" s="129"/>
-      <c r="K28" s="129"/>
-      <c r="L28" s="129"/>
-      <c r="M28" s="129"/>
-      <c r="N28" s="129"/>
-      <c r="O28" s="129"/>
+      <c r="G28" s="119"/>
+      <c r="H28" s="114"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="115"/>
+      <c r="K28" s="115"/>
+      <c r="L28" s="115"/>
+      <c r="M28" s="115"/>
+      <c r="N28" s="115"/>
+      <c r="O28" s="115"/>
       <c r="P28" s="77"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.35">
@@ -6007,34 +6015,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:O25"/>
-    <mergeCell ref="H27:O28"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:O22"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="S4:S6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="N4:N6"/>
     <mergeCell ref="AK4:AK6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
@@ -6051,6 +6031,34 @@
     <mergeCell ref="W4:W6"/>
     <mergeCell ref="X4:X6"/>
     <mergeCell ref="O4:O6"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="Q4:Q6"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:O25"/>
+    <mergeCell ref="H27:O28"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:O22"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" verticalDpi="1200" r:id="rId1"/>
@@ -6187,64 +6195,64 @@
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="71"/>
-      <c r="E4" s="121" t="s">
+      <c r="E4" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="G4" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="118" t="s">
+      <c r="H4" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="118" t="s">
+      <c r="I4" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="118" t="s">
+      <c r="J4" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="118" t="s">
+      <c r="K4" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="118" t="s">
+      <c r="L4" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="115" t="s">
+      <c r="M4" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="115" t="s">
+      <c r="N4" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="115" t="s">
+      <c r="O4" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="115" t="s">
+      <c r="P4" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="115" t="s">
+      <c r="Q4" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="115" t="s">
+      <c r="R4" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="115" t="s">
+      <c r="S4" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="106" t="s">
+      <c r="T4" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="106" t="s">
+      <c r="U4" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="106" t="s">
+      <c r="V4" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="W4" s="109" t="s">
+      <c r="W4" s="145" t="s">
         <v>21</v>
       </c>
-      <c r="X4" s="112" t="s">
+      <c r="X4" s="148" t="s">
         <v>22</v>
       </c>
       <c r="Y4" s="65"/>
@@ -6254,22 +6262,22 @@
       <c r="AC4" s="66"/>
       <c r="AD4" s="66"/>
       <c r="AE4" s="67"/>
-      <c r="AF4" s="100" t="s">
+      <c r="AF4" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="AG4" s="103" t="s">
+      <c r="AG4" s="139" t="s">
         <v>24</v>
       </c>
-      <c r="AH4" s="103" t="s">
+      <c r="AH4" s="139" t="s">
         <v>25</v>
       </c>
-      <c r="AI4" s="103" t="s">
+      <c r="AI4" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="AJ4" s="103" t="s">
+      <c r="AJ4" s="139" t="s">
         <v>27</v>
       </c>
-      <c r="AK4" s="91" t="s">
+      <c r="AK4" s="129" t="s">
         <v>28</v>
       </c>
     </row>
@@ -6279,26 +6287,26 @@
       </c>
       <c r="C5" s="60"/>
       <c r="D5" s="63"/>
-      <c r="E5" s="122"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="113"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="124"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="127"/>
+      <c r="N5" s="127"/>
+      <c r="O5" s="127"/>
+      <c r="P5" s="127"/>
+      <c r="Q5" s="127"/>
+      <c r="R5" s="127"/>
+      <c r="S5" s="127"/>
+      <c r="T5" s="143"/>
+      <c r="U5" s="143"/>
+      <c r="V5" s="143"/>
+      <c r="W5" s="146"/>
+      <c r="X5" s="149"/>
       <c r="Y5" s="68"/>
       <c r="Z5" s="69"/>
       <c r="AA5" s="69"/>
@@ -6306,37 +6314,37 @@
       <c r="AC5" s="69"/>
       <c r="AD5" s="69"/>
       <c r="AE5" s="70"/>
-      <c r="AF5" s="101"/>
-      <c r="AG5" s="104"/>
-      <c r="AH5" s="104"/>
-      <c r="AI5" s="104"/>
-      <c r="AJ5" s="104"/>
-      <c r="AK5" s="92"/>
+      <c r="AF5" s="137"/>
+      <c r="AG5" s="140"/>
+      <c r="AH5" s="140"/>
+      <c r="AI5" s="140"/>
+      <c r="AJ5" s="140"/>
+      <c r="AK5" s="130"/>
     </row>
     <row r="6" spans="2:37" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="38"/>
       <c r="C6" s="64"/>
       <c r="D6" s="34"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="108"/>
-      <c r="U6" s="108"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="111"/>
-      <c r="X6" s="114"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="125"/>
+      <c r="M6" s="128"/>
+      <c r="N6" s="128"/>
+      <c r="O6" s="128"/>
+      <c r="P6" s="128"/>
+      <c r="Q6" s="128"/>
+      <c r="R6" s="128"/>
+      <c r="S6" s="128"/>
+      <c r="T6" s="144"/>
+      <c r="U6" s="144"/>
+      <c r="V6" s="144"/>
+      <c r="W6" s="147"/>
+      <c r="X6" s="150"/>
       <c r="Y6" s="72" t="s">
         <v>30</v>
       </c>
@@ -6358,21 +6366,21 @@
       <c r="AE6" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="AF6" s="102"/>
-      <c r="AG6" s="105"/>
-      <c r="AH6" s="105"/>
-      <c r="AI6" s="105"/>
-      <c r="AJ6" s="105"/>
-      <c r="AK6" s="93"/>
+      <c r="AF6" s="138"/>
+      <c r="AG6" s="141"/>
+      <c r="AH6" s="141"/>
+      <c r="AI6" s="141"/>
+      <c r="AJ6" s="141"/>
+      <c r="AK6" s="131"/>
     </row>
     <row r="7" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="150" t="s">
+      <c r="C7" s="155" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="151"/>
+      <c r="D7" s="156"/>
       <c r="E7" s="40"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
@@ -6408,11 +6416,11 @@
       <c r="AK7" s="7"/>
     </row>
     <row r="8" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="138"/>
-      <c r="C8" s="152" t="s">
+      <c r="B8" s="96"/>
+      <c r="C8" s="157" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="153"/>
+      <c r="D8" s="158"/>
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -6448,11 +6456,11 @@
       <c r="AK8" s="9"/>
     </row>
     <row r="9" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="138"/>
-      <c r="C9" s="154" t="s">
+      <c r="B9" s="96"/>
+      <c r="C9" s="159" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="155"/>
+      <c r="D9" s="160"/>
       <c r="E9" s="45"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -6488,11 +6496,11 @@
       <c r="AK9" s="9"/>
     </row>
     <row r="10" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="138"/>
-      <c r="C10" s="154" t="s">
+      <c r="B10" s="96"/>
+      <c r="C10" s="159" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="155"/>
+      <c r="D10" s="160"/>
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -6528,11 +6536,11 @@
       <c r="AK10" s="9"/>
     </row>
     <row r="11" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="138"/>
-      <c r="C11" s="154" t="s">
+      <c r="B11" s="96"/>
+      <c r="C11" s="159" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="155"/>
+      <c r="D11" s="160"/>
       <c r="E11" s="15"/>
       <c r="F11" s="44"/>
       <c r="G11" s="14"/>
@@ -6568,11 +6576,11 @@
       <c r="AK11" s="9"/>
     </row>
     <row r="12" spans="2:37" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="139"/>
-      <c r="C12" s="156" t="s">
+      <c r="B12" s="97"/>
+      <c r="C12" s="161" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="157"/>
+      <c r="D12" s="162"/>
       <c r="E12" s="46"/>
       <c r="F12" s="47"/>
       <c r="G12" s="47"/>
@@ -6608,13 +6616,13 @@
       <c r="AK12" s="18"/>
     </row>
     <row r="13" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B13" s="134" t="s">
+      <c r="B13" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="158" t="s">
+      <c r="C13" s="151" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="159"/>
+      <c r="D13" s="152"/>
       <c r="E13" s="62"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
@@ -6650,11 +6658,11 @@
       <c r="AK13" s="27"/>
     </row>
     <row r="14" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B14" s="135"/>
-      <c r="C14" s="160" t="s">
+      <c r="B14" s="93"/>
+      <c r="C14" s="153" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="161"/>
+      <c r="D14" s="154"/>
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
@@ -6690,11 +6698,11 @@
       <c r="AK14" s="28"/>
     </row>
     <row r="15" spans="2:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B15" s="135"/>
-      <c r="C15" s="146" t="s">
+      <c r="B15" s="93"/>
+      <c r="C15" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="147"/>
+      <c r="D15" s="107"/>
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
@@ -6730,11 +6738,11 @@
       <c r="AK15" s="28"/>
     </row>
     <row r="16" spans="2:37" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="B16" s="136"/>
-      <c r="C16" s="148" t="s">
+      <c r="B16" s="94"/>
+      <c r="C16" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="149"/>
+      <c r="D16" s="109"/>
       <c r="E16" s="29"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
@@ -6771,11 +6779,23 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="T4:T6"/>
+    <mergeCell ref="U4:U6"/>
+    <mergeCell ref="V4:V6"/>
     <mergeCell ref="AJ4:AJ6"/>
     <mergeCell ref="AK4:AK6"/>
     <mergeCell ref="B7:B12"/>
@@ -6792,23 +6812,11 @@
     <mergeCell ref="AH4:AH6"/>
     <mergeCell ref="AI4:AI6"/>
     <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="S4:S6"/>
-    <mergeCell ref="T4:T6"/>
-    <mergeCell ref="U4:U6"/>
-    <mergeCell ref="V4:V6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="N4:N6"/>
-    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6827,351 +6835,351 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="163" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
-      <c r="K2" s="162"/>
-      <c r="L2" s="162"/>
-      <c r="M2" s="162"/>
-      <c r="N2" s="162"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
+      <c r="J2" s="163"/>
+      <c r="K2" s="163"/>
+      <c r="L2" s="163"/>
+      <c r="M2" s="163"/>
+      <c r="N2" s="163"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B3" s="163"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="163"/>
-      <c r="I3" s="163"/>
-      <c r="J3" s="163"/>
-      <c r="K3" s="163"/>
-      <c r="L3" s="163"/>
-      <c r="M3" s="163"/>
-      <c r="N3" s="163"/>
+      <c r="B3" s="164"/>
+      <c r="C3" s="164"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="164"/>
+      <c r="F3" s="164"/>
+      <c r="G3" s="164"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="164"/>
+      <c r="J3" s="164"/>
+      <c r="K3" s="164"/>
+      <c r="L3" s="164"/>
+      <c r="M3" s="164"/>
+      <c r="N3" s="164"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B4" s="163"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="163"/>
-      <c r="J4" s="163"/>
-      <c r="K4" s="163"/>
-      <c r="L4" s="163"/>
-      <c r="M4" s="163"/>
-      <c r="N4" s="163"/>
+      <c r="B4" s="164"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="164"/>
+      <c r="F4" s="164"/>
+      <c r="G4" s="164"/>
+      <c r="H4" s="164"/>
+      <c r="I4" s="164"/>
+      <c r="J4" s="164"/>
+      <c r="K4" s="164"/>
+      <c r="L4" s="164"/>
+      <c r="M4" s="164"/>
+      <c r="N4" s="164"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="163"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="163"/>
-      <c r="H5" s="163"/>
-      <c r="I5" s="163"/>
-      <c r="J5" s="163"/>
-      <c r="K5" s="163"/>
-      <c r="L5" s="163"/>
-      <c r="M5" s="163"/>
-      <c r="N5" s="163"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
+      <c r="F5" s="164"/>
+      <c r="G5" s="164"/>
+      <c r="H5" s="164"/>
+      <c r="I5" s="164"/>
+      <c r="J5" s="164"/>
+      <c r="K5" s="164"/>
+      <c r="L5" s="164"/>
+      <c r="M5" s="164"/>
+      <c r="N5" s="164"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="163"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="163"/>
-      <c r="J6" s="163"/>
-      <c r="K6" s="163"/>
-      <c r="L6" s="163"/>
-      <c r="M6" s="163"/>
-      <c r="N6" s="163"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="164"/>
+      <c r="D6" s="164"/>
+      <c r="E6" s="164"/>
+      <c r="F6" s="164"/>
+      <c r="G6" s="164"/>
+      <c r="H6" s="164"/>
+      <c r="I6" s="164"/>
+      <c r="J6" s="164"/>
+      <c r="K6" s="164"/>
+      <c r="L6" s="164"/>
+      <c r="M6" s="164"/>
+      <c r="N6" s="164"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="163"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="163"/>
-      <c r="H7" s="163"/>
-      <c r="I7" s="163"/>
-      <c r="J7" s="163"/>
-      <c r="K7" s="163"/>
-      <c r="L7" s="163"/>
-      <c r="M7" s="163"/>
-      <c r="N7" s="163"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="164"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
+      <c r="H7" s="164"/>
+      <c r="I7" s="164"/>
+      <c r="J7" s="164"/>
+      <c r="K7" s="164"/>
+      <c r="L7" s="164"/>
+      <c r="M7" s="164"/>
+      <c r="N7" s="164"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="163"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="163"/>
-      <c r="H8" s="163"/>
-      <c r="I8" s="163"/>
-      <c r="J8" s="163"/>
-      <c r="K8" s="163"/>
-      <c r="L8" s="163"/>
-      <c r="M8" s="163"/>
-      <c r="N8" s="163"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="164"/>
+      <c r="D8" s="164"/>
+      <c r="E8" s="164"/>
+      <c r="F8" s="164"/>
+      <c r="G8" s="164"/>
+      <c r="H8" s="164"/>
+      <c r="I8" s="164"/>
+      <c r="J8" s="164"/>
+      <c r="K8" s="164"/>
+      <c r="L8" s="164"/>
+      <c r="M8" s="164"/>
+      <c r="N8" s="164"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="163"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="163"/>
-      <c r="H9" s="163"/>
-      <c r="I9" s="163"/>
-      <c r="J9" s="163"/>
-      <c r="K9" s="163"/>
-      <c r="L9" s="163"/>
-      <c r="M9" s="163"/>
-      <c r="N9" s="163"/>
+      <c r="B9" s="164"/>
+      <c r="C9" s="164"/>
+      <c r="D9" s="164"/>
+      <c r="E9" s="164"/>
+      <c r="F9" s="164"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="164"/>
+      <c r="I9" s="164"/>
+      <c r="J9" s="164"/>
+      <c r="K9" s="164"/>
+      <c r="L9" s="164"/>
+      <c r="M9" s="164"/>
+      <c r="N9" s="164"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="163"/>
-      <c r="C10" s="163"/>
-      <c r="D10" s="163"/>
-      <c r="E10" s="163"/>
-      <c r="F10" s="163"/>
-      <c r="G10" s="163"/>
-      <c r="H10" s="163"/>
-      <c r="I10" s="163"/>
-      <c r="J10" s="163"/>
-      <c r="K10" s="163"/>
-      <c r="L10" s="163"/>
-      <c r="M10" s="163"/>
-      <c r="N10" s="163"/>
+      <c r="B10" s="164"/>
+      <c r="C10" s="164"/>
+      <c r="D10" s="164"/>
+      <c r="E10" s="164"/>
+      <c r="F10" s="164"/>
+      <c r="G10" s="164"/>
+      <c r="H10" s="164"/>
+      <c r="I10" s="164"/>
+      <c r="J10" s="164"/>
+      <c r="K10" s="164"/>
+      <c r="L10" s="164"/>
+      <c r="M10" s="164"/>
+      <c r="N10" s="164"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B11" s="163"/>
-      <c r="C11" s="163"/>
-      <c r="D11" s="163"/>
-      <c r="E11" s="163"/>
-      <c r="F11" s="163"/>
-      <c r="G11" s="163"/>
-      <c r="H11" s="163"/>
-      <c r="I11" s="163"/>
-      <c r="J11" s="163"/>
-      <c r="K11" s="163"/>
-      <c r="L11" s="163"/>
-      <c r="M11" s="163"/>
-      <c r="N11" s="163"/>
+      <c r="B11" s="164"/>
+      <c r="C11" s="164"/>
+      <c r="D11" s="164"/>
+      <c r="E11" s="164"/>
+      <c r="F11" s="164"/>
+      <c r="G11" s="164"/>
+      <c r="H11" s="164"/>
+      <c r="I11" s="164"/>
+      <c r="J11" s="164"/>
+      <c r="K11" s="164"/>
+      <c r="L11" s="164"/>
+      <c r="M11" s="164"/>
+      <c r="N11" s="164"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B12" s="163"/>
-      <c r="C12" s="163"/>
-      <c r="D12" s="163"/>
-      <c r="E12" s="163"/>
-      <c r="F12" s="163"/>
-      <c r="G12" s="163"/>
-      <c r="H12" s="163"/>
-      <c r="I12" s="163"/>
-      <c r="J12" s="163"/>
-      <c r="K12" s="163"/>
-      <c r="L12" s="163"/>
-      <c r="M12" s="163"/>
-      <c r="N12" s="163"/>
+      <c r="B12" s="164"/>
+      <c r="C12" s="164"/>
+      <c r="D12" s="164"/>
+      <c r="E12" s="164"/>
+      <c r="F12" s="164"/>
+      <c r="G12" s="164"/>
+      <c r="H12" s="164"/>
+      <c r="I12" s="164"/>
+      <c r="J12" s="164"/>
+      <c r="K12" s="164"/>
+      <c r="L12" s="164"/>
+      <c r="M12" s="164"/>
+      <c r="N12" s="164"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="163"/>
-      <c r="C13" s="163"/>
-      <c r="D13" s="163"/>
-      <c r="E13" s="163"/>
-      <c r="F13" s="163"/>
-      <c r="G13" s="163"/>
-      <c r="H13" s="163"/>
-      <c r="I13" s="163"/>
-      <c r="J13" s="163"/>
-      <c r="K13" s="163"/>
-      <c r="L13" s="163"/>
-      <c r="M13" s="163"/>
-      <c r="N13" s="163"/>
+      <c r="B13" s="164"/>
+      <c r="C13" s="164"/>
+      <c r="D13" s="164"/>
+      <c r="E13" s="164"/>
+      <c r="F13" s="164"/>
+      <c r="G13" s="164"/>
+      <c r="H13" s="164"/>
+      <c r="I13" s="164"/>
+      <c r="J13" s="164"/>
+      <c r="K13" s="164"/>
+      <c r="L13" s="164"/>
+      <c r="M13" s="164"/>
+      <c r="N13" s="164"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="163"/>
-      <c r="C14" s="163"/>
-      <c r="D14" s="163"/>
-      <c r="E14" s="163"/>
-      <c r="F14" s="163"/>
-      <c r="G14" s="163"/>
-      <c r="H14" s="163"/>
-      <c r="I14" s="163"/>
-      <c r="J14" s="163"/>
-      <c r="K14" s="163"/>
-      <c r="L14" s="163"/>
-      <c r="M14" s="163"/>
-      <c r="N14" s="163"/>
+      <c r="B14" s="164"/>
+      <c r="C14" s="164"/>
+      <c r="D14" s="164"/>
+      <c r="E14" s="164"/>
+      <c r="F14" s="164"/>
+      <c r="G14" s="164"/>
+      <c r="H14" s="164"/>
+      <c r="I14" s="164"/>
+      <c r="J14" s="164"/>
+      <c r="K14" s="164"/>
+      <c r="L14" s="164"/>
+      <c r="M14" s="164"/>
+      <c r="N14" s="164"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="163"/>
-      <c r="C15" s="163"/>
-      <c r="D15" s="163"/>
-      <c r="E15" s="163"/>
-      <c r="F15" s="163"/>
-      <c r="G15" s="163"/>
-      <c r="H15" s="163"/>
-      <c r="I15" s="163"/>
-      <c r="J15" s="163"/>
-      <c r="K15" s="163"/>
-      <c r="L15" s="163"/>
-      <c r="M15" s="163"/>
-      <c r="N15" s="163"/>
+      <c r="B15" s="164"/>
+      <c r="C15" s="164"/>
+      <c r="D15" s="164"/>
+      <c r="E15" s="164"/>
+      <c r="F15" s="164"/>
+      <c r="G15" s="164"/>
+      <c r="H15" s="164"/>
+      <c r="I15" s="164"/>
+      <c r="J15" s="164"/>
+      <c r="K15" s="164"/>
+      <c r="L15" s="164"/>
+      <c r="M15" s="164"/>
+      <c r="N15" s="164"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B16" s="163"/>
-      <c r="C16" s="163"/>
-      <c r="D16" s="163"/>
-      <c r="E16" s="163"/>
-      <c r="F16" s="163"/>
-      <c r="G16" s="163"/>
-      <c r="H16" s="163"/>
-      <c r="I16" s="163"/>
-      <c r="J16" s="163"/>
-      <c r="K16" s="163"/>
-      <c r="L16" s="163"/>
-      <c r="M16" s="163"/>
-      <c r="N16" s="163"/>
+      <c r="B16" s="164"/>
+      <c r="C16" s="164"/>
+      <c r="D16" s="164"/>
+      <c r="E16" s="164"/>
+      <c r="F16" s="164"/>
+      <c r="G16" s="164"/>
+      <c r="H16" s="164"/>
+      <c r="I16" s="164"/>
+      <c r="J16" s="164"/>
+      <c r="K16" s="164"/>
+      <c r="L16" s="164"/>
+      <c r="M16" s="164"/>
+      <c r="N16" s="164"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B17" s="163"/>
-      <c r="C17" s="163"/>
-      <c r="D17" s="163"/>
-      <c r="E17" s="163"/>
-      <c r="F17" s="163"/>
-      <c r="G17" s="163"/>
-      <c r="H17" s="163"/>
-      <c r="I17" s="163"/>
-      <c r="J17" s="163"/>
-      <c r="K17" s="163"/>
-      <c r="L17" s="163"/>
-      <c r="M17" s="163"/>
-      <c r="N17" s="163"/>
+      <c r="B17" s="164"/>
+      <c r="C17" s="164"/>
+      <c r="D17" s="164"/>
+      <c r="E17" s="164"/>
+      <c r="F17" s="164"/>
+      <c r="G17" s="164"/>
+      <c r="H17" s="164"/>
+      <c r="I17" s="164"/>
+      <c r="J17" s="164"/>
+      <c r="K17" s="164"/>
+      <c r="L17" s="164"/>
+      <c r="M17" s="164"/>
+      <c r="N17" s="164"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B18" s="163"/>
-      <c r="C18" s="163"/>
-      <c r="D18" s="163"/>
-      <c r="E18" s="163"/>
-      <c r="F18" s="163"/>
-      <c r="G18" s="163"/>
-      <c r="H18" s="163"/>
-      <c r="I18" s="163"/>
-      <c r="J18" s="163"/>
-      <c r="K18" s="163"/>
-      <c r="L18" s="163"/>
-      <c r="M18" s="163"/>
-      <c r="N18" s="163"/>
+      <c r="B18" s="164"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="164"/>
+      <c r="H18" s="164"/>
+      <c r="I18" s="164"/>
+      <c r="J18" s="164"/>
+      <c r="K18" s="164"/>
+      <c r="L18" s="164"/>
+      <c r="M18" s="164"/>
+      <c r="N18" s="164"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B19" s="163"/>
-      <c r="C19" s="163"/>
-      <c r="D19" s="163"/>
-      <c r="E19" s="163"/>
-      <c r="F19" s="163"/>
-      <c r="G19" s="163"/>
-      <c r="H19" s="163"/>
-      <c r="I19" s="163"/>
-      <c r="J19" s="163"/>
-      <c r="K19" s="163"/>
-      <c r="L19" s="163"/>
-      <c r="M19" s="163"/>
-      <c r="N19" s="163"/>
+      <c r="B19" s="164"/>
+      <c r="C19" s="164"/>
+      <c r="D19" s="164"/>
+      <c r="E19" s="164"/>
+      <c r="F19" s="164"/>
+      <c r="G19" s="164"/>
+      <c r="H19" s="164"/>
+      <c r="I19" s="164"/>
+      <c r="J19" s="164"/>
+      <c r="K19" s="164"/>
+      <c r="L19" s="164"/>
+      <c r="M19" s="164"/>
+      <c r="N19" s="164"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B20" s="163"/>
-      <c r="C20" s="163"/>
-      <c r="D20" s="163"/>
-      <c r="E20" s="163"/>
-      <c r="F20" s="163"/>
-      <c r="G20" s="163"/>
-      <c r="H20" s="163"/>
-      <c r="I20" s="163"/>
-      <c r="J20" s="163"/>
-      <c r="K20" s="163"/>
-      <c r="L20" s="163"/>
-      <c r="M20" s="163"/>
-      <c r="N20" s="163"/>
+      <c r="B20" s="164"/>
+      <c r="C20" s="164"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="164"/>
+      <c r="F20" s="164"/>
+      <c r="G20" s="164"/>
+      <c r="H20" s="164"/>
+      <c r="I20" s="164"/>
+      <c r="J20" s="164"/>
+      <c r="K20" s="164"/>
+      <c r="L20" s="164"/>
+      <c r="M20" s="164"/>
+      <c r="N20" s="164"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B21" s="163"/>
-      <c r="C21" s="163"/>
-      <c r="D21" s="163"/>
-      <c r="E21" s="163"/>
-      <c r="F21" s="163"/>
-      <c r="G21" s="163"/>
-      <c r="H21" s="163"/>
-      <c r="I21" s="163"/>
-      <c r="J21" s="163"/>
-      <c r="K21" s="163"/>
-      <c r="L21" s="163"/>
-      <c r="M21" s="163"/>
-      <c r="N21" s="163"/>
+      <c r="B21" s="164"/>
+      <c r="C21" s="164"/>
+      <c r="D21" s="164"/>
+      <c r="E21" s="164"/>
+      <c r="F21" s="164"/>
+      <c r="G21" s="164"/>
+      <c r="H21" s="164"/>
+      <c r="I21" s="164"/>
+      <c r="J21" s="164"/>
+      <c r="K21" s="164"/>
+      <c r="L21" s="164"/>
+      <c r="M21" s="164"/>
+      <c r="N21" s="164"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B22" s="163"/>
-      <c r="C22" s="163"/>
-      <c r="D22" s="163"/>
-      <c r="E22" s="163"/>
-      <c r="F22" s="163"/>
-      <c r="G22" s="163"/>
-      <c r="H22" s="163"/>
-      <c r="I22" s="163"/>
-      <c r="J22" s="163"/>
-      <c r="K22" s="163"/>
-      <c r="L22" s="163"/>
-      <c r="M22" s="163"/>
-      <c r="N22" s="163"/>
+      <c r="B22" s="164"/>
+      <c r="C22" s="164"/>
+      <c r="D22" s="164"/>
+      <c r="E22" s="164"/>
+      <c r="F22" s="164"/>
+      <c r="G22" s="164"/>
+      <c r="H22" s="164"/>
+      <c r="I22" s="164"/>
+      <c r="J22" s="164"/>
+      <c r="K22" s="164"/>
+      <c r="L22" s="164"/>
+      <c r="M22" s="164"/>
+      <c r="N22" s="164"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="163"/>
-      <c r="C23" s="163"/>
-      <c r="D23" s="163"/>
-      <c r="E23" s="163"/>
-      <c r="F23" s="163"/>
-      <c r="G23" s="163"/>
-      <c r="H23" s="163"/>
-      <c r="I23" s="163"/>
-      <c r="J23" s="163"/>
-      <c r="K23" s="163"/>
-      <c r="L23" s="163"/>
-      <c r="M23" s="163"/>
-      <c r="N23" s="163"/>
+      <c r="B23" s="164"/>
+      <c r="C23" s="164"/>
+      <c r="D23" s="164"/>
+      <c r="E23" s="164"/>
+      <c r="F23" s="164"/>
+      <c r="G23" s="164"/>
+      <c r="H23" s="164"/>
+      <c r="I23" s="164"/>
+      <c r="J23" s="164"/>
+      <c r="K23" s="164"/>
+      <c r="L23" s="164"/>
+      <c r="M23" s="164"/>
+      <c r="N23" s="164"/>
     </row>
     <row r="24" spans="2:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="163"/>
-      <c r="C24" s="163"/>
-      <c r="D24" s="163"/>
-      <c r="E24" s="163"/>
-      <c r="F24" s="163"/>
-      <c r="G24" s="163"/>
-      <c r="H24" s="163"/>
-      <c r="I24" s="163"/>
-      <c r="J24" s="163"/>
-      <c r="K24" s="163"/>
-      <c r="L24" s="163"/>
-      <c r="M24" s="163"/>
-      <c r="N24" s="163"/>
+      <c r="B24" s="164"/>
+      <c r="C24" s="164"/>
+      <c r="D24" s="164"/>
+      <c r="E24" s="164"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="164"/>
+      <c r="H24" s="164"/>
+      <c r="I24" s="164"/>
+      <c r="J24" s="164"/>
+      <c r="K24" s="164"/>
+      <c r="L24" s="164"/>
+      <c r="M24" s="164"/>
+      <c r="N24" s="164"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7182,6 +7190,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="cc018f0f-33de-4c4c-920d-26dc6e1acc33" xsi:nil="true"/>
+    <test xmlns="8e39aab0-005d-45b6-a80e-05e5df2908d1" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8e39aab0-005d-45b6-a80e-05e5df2908d1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010081A80706761E274FBF7207A6EEFD509E" ma:contentTypeVersion="20" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="a00a05fe2e076f083d323378c5165ffd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8e39aab0-005d-45b6-a80e-05e5df2908d1" xmlns:ns3="cc018f0f-33de-4c4c-920d-26dc6e1acc33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64bb212a3759e4adb139958771eb6e76" ns2:_="" ns3:_="">
     <xsd:import namespace="8e39aab0-005d-45b6-a80e-05e5df2908d1"/>
@@ -7444,28 +7473,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA41F33-D73A-4946-89E5-437EF57CC713}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cc018f0f-33de-4c4c-920d-26dc6e1acc33"/>
+    <ds:schemaRef ds:uri="8e39aab0-005d-45b6-a80e-05e5df2908d1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="cc018f0f-33de-4c4c-920d-26dc6e1acc33" xsi:nil="true"/>
-    <test xmlns="8e39aab0-005d-45b6-a80e-05e5df2908d1" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8e39aab0-005d-45b6-a80e-05e5df2908d1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FEB2382-117C-4B02-B61B-7207F73C69D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF0F5F45-92AD-4EE8-ADF4-74DBCD118A57}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7482,23 +7509,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FEB2382-117C-4B02-B61B-7207F73C69D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA41F33-D73A-4946-89E5-437EF57CC713}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cc018f0f-33de-4c4c-920d-26dc6e1acc33"/>
-    <ds:schemaRef ds:uri="8e39aab0-005d-45b6-a80e-05e5df2908d1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>